<commit_message>
Re-Run Adam and SR-Adam for model saving
</commit_message>
<xml_diff>
--- a/results/CIFAR10/simplecnn/noise_0.0/Adam/runs_and_aggregate.xlsx
+++ b/results/CIFAR10/simplecnn/noise_0.0/Adam/runs_and_aggregate.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="run_1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="run_2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="run_3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="run_4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="run_5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="aggregate" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="run_1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="run_2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="run_3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="run_4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="run_5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="aggregate" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -487,7 +487,7 @@
         <v>48.2</v>
       </c>
       <c r="F2" t="n">
-        <v>33.30055141448975</v>
+        <v>33.17258048057556</v>
       </c>
     </row>
     <row r="3">
@@ -507,7 +507,7 @@
         <v>55.86</v>
       </c>
       <c r="F3" t="n">
-        <v>34.45650720596313</v>
+        <v>32.05534434318542</v>
       </c>
     </row>
     <row r="4">
@@ -527,7 +527,7 @@
         <v>59.45</v>
       </c>
       <c r="F4" t="n">
-        <v>32.71675777435303</v>
+        <v>30.90100288391113</v>
       </c>
     </row>
     <row r="5">
@@ -547,7 +547,7 @@
         <v>62.58</v>
       </c>
       <c r="F5" t="n">
-        <v>32.63468289375305</v>
+        <v>28.24356484413147</v>
       </c>
     </row>
     <row r="6">
@@ -567,7 +567,7 @@
         <v>64.84</v>
       </c>
       <c r="F6" t="n">
-        <v>32.77680611610413</v>
+        <v>26.69353222846985</v>
       </c>
     </row>
     <row r="7">
@@ -587,7 +587,7 @@
         <v>67.18000000000001</v>
       </c>
       <c r="F7" t="n">
-        <v>32.77470111846924</v>
+        <v>26.29553723335266</v>
       </c>
     </row>
     <row r="8">
@@ -607,7 +607,7 @@
         <v>68.90000000000001</v>
       </c>
       <c r="F8" t="n">
-        <v>32.49112057685852</v>
+        <v>26.31389260292053</v>
       </c>
     </row>
     <row r="9">
@@ -627,7 +627,7 @@
         <v>68.72</v>
       </c>
       <c r="F9" t="n">
-        <v>32.55548405647278</v>
+        <v>26.31670951843262</v>
       </c>
     </row>
     <row r="10">
@@ -647,7 +647,7 @@
         <v>70.23999999999999</v>
       </c>
       <c r="F10" t="n">
-        <v>32.82826900482178</v>
+        <v>26.22270464897156</v>
       </c>
     </row>
     <row r="11">
@@ -667,7 +667,7 @@
         <v>70.63</v>
       </c>
       <c r="F11" t="n">
-        <v>33.89722657203674</v>
+        <v>26.42997121810913</v>
       </c>
     </row>
     <row r="12">
@@ -687,7 +687,7 @@
         <v>70.54000000000001</v>
       </c>
       <c r="F12" t="n">
-        <v>33.58312392234802</v>
+        <v>26.50774264335632</v>
       </c>
     </row>
     <row r="13">
@@ -707,7 +707,7 @@
         <v>71.94</v>
       </c>
       <c r="F13" t="n">
-        <v>33.02881288528442</v>
+        <v>26.34843826293945</v>
       </c>
     </row>
     <row r="14">
@@ -727,7 +727,7 @@
         <v>72.23999999999999</v>
       </c>
       <c r="F14" t="n">
-        <v>34.13583469390869</v>
+        <v>26.39791345596313</v>
       </c>
     </row>
     <row r="15">
@@ -747,7 +747,7 @@
         <v>73.38</v>
       </c>
       <c r="F15" t="n">
-        <v>32.6794331073761</v>
+        <v>26.6412320137024</v>
       </c>
     </row>
     <row r="16">
@@ -767,7 +767,7 @@
         <v>73.72</v>
       </c>
       <c r="F16" t="n">
-        <v>32.60413765907288</v>
+        <v>26.5207884311676</v>
       </c>
     </row>
     <row r="17">
@@ -787,7 +787,7 @@
         <v>73.97</v>
       </c>
       <c r="F17" t="n">
-        <v>32.66315054893494</v>
+        <v>26.52726316452026</v>
       </c>
     </row>
     <row r="18">
@@ -807,7 +807,7 @@
         <v>73.06</v>
       </c>
       <c r="F18" t="n">
-        <v>33.76850843429565</v>
+        <v>26.46880984306335</v>
       </c>
     </row>
     <row r="19">
@@ -827,7 +827,7 @@
         <v>74.8</v>
       </c>
       <c r="F19" t="n">
-        <v>32.75617241859436</v>
+        <v>26.51732516288757</v>
       </c>
     </row>
     <row r="20">
@@ -847,7 +847,7 @@
         <v>74.47</v>
       </c>
       <c r="F20" t="n">
-        <v>32.65529680252075</v>
+        <v>26.51289939880371</v>
       </c>
     </row>
     <row r="21">
@@ -867,7 +867,7 @@
         <v>75.11</v>
       </c>
       <c r="F21" t="n">
-        <v>32.61110544204712</v>
+        <v>26.75679087638855</v>
       </c>
     </row>
   </sheetData>
@@ -938,7 +938,7 @@
         <v>48.24</v>
       </c>
       <c r="F2" t="n">
-        <v>32.84016108512878</v>
+        <v>26.71737504005432</v>
       </c>
     </row>
     <row r="3">
@@ -958,7 +958,7 @@
         <v>54.9</v>
       </c>
       <c r="F3" t="n">
-        <v>32.96483397483826</v>
+        <v>26.37820482254028</v>
       </c>
     </row>
     <row r="4">
@@ -978,7 +978,7 @@
         <v>58.73</v>
       </c>
       <c r="F4" t="n">
-        <v>32.94972586631775</v>
+        <v>26.44888615608216</v>
       </c>
     </row>
     <row r="5">
@@ -998,7 +998,7 @@
         <v>62.3</v>
       </c>
       <c r="F5" t="n">
-        <v>32.80088949203491</v>
+        <v>26.38553357124329</v>
       </c>
     </row>
     <row r="6">
@@ -1018,7 +1018,7 @@
         <v>63.37</v>
       </c>
       <c r="F6" t="n">
-        <v>33.55512118339539</v>
+        <v>26.44520020484924</v>
       </c>
     </row>
     <row r="7">
@@ -1038,7 +1038,7 @@
         <v>64.91</v>
       </c>
       <c r="F7" t="n">
-        <v>32.9557900428772</v>
+        <v>26.45350241661072</v>
       </c>
     </row>
     <row r="8">
@@ -1058,7 +1058,7 @@
         <v>66.34</v>
       </c>
       <c r="F8" t="n">
-        <v>32.77284264564514</v>
+        <v>26.4281108379364</v>
       </c>
     </row>
     <row r="9">
@@ -1078,7 +1078,7 @@
         <v>66.83</v>
       </c>
       <c r="F9" t="n">
-        <v>33.90411162376404</v>
+        <v>26.42350506782532</v>
       </c>
     </row>
     <row r="10">
@@ -1098,7 +1098,7 @@
         <v>68.58</v>
       </c>
       <c r="F10" t="n">
-        <v>33.97514176368713</v>
+        <v>26.52731561660766</v>
       </c>
     </row>
     <row r="11">
@@ -1118,7 +1118,7 @@
         <v>70.03</v>
       </c>
       <c r="F11" t="n">
-        <v>33.82056832313538</v>
+        <v>26.74628043174744</v>
       </c>
     </row>
     <row r="12">
@@ -1138,7 +1138,7 @@
         <v>69.41</v>
       </c>
       <c r="F12" t="n">
-        <v>33.97257423400879</v>
+        <v>26.55410480499268</v>
       </c>
     </row>
     <row r="13">
@@ -1158,7 +1158,7 @@
         <v>71.23999999999999</v>
       </c>
       <c r="F13" t="n">
-        <v>32.84733271598816</v>
+        <v>26.46813440322876</v>
       </c>
     </row>
     <row r="14">
@@ -1178,7 +1178,7 @@
         <v>71.08</v>
       </c>
       <c r="F14" t="n">
-        <v>32.71444058418274</v>
+        <v>26.52019357681274</v>
       </c>
     </row>
     <row r="15">
@@ -1198,7 +1198,7 @@
         <v>71.78</v>
       </c>
       <c r="F15" t="n">
-        <v>33.70076322555542</v>
+        <v>26.62460660934448</v>
       </c>
     </row>
     <row r="16">
@@ -1218,7 +1218,7 @@
         <v>71.52</v>
       </c>
       <c r="F16" t="n">
-        <v>33.00230741500854</v>
+        <v>26.59368944168091</v>
       </c>
     </row>
     <row r="17">
@@ -1238,7 +1238,7 @@
         <v>72.67</v>
       </c>
       <c r="F17" t="n">
-        <v>33.2676203250885</v>
+        <v>26.72600412368774</v>
       </c>
     </row>
     <row r="18">
@@ -1258,7 +1258,7 @@
         <v>72.67</v>
       </c>
       <c r="F18" t="n">
-        <v>33.35620975494385</v>
+        <v>26.6620180606842</v>
       </c>
     </row>
     <row r="19">
@@ -1278,7 +1278,7 @@
         <v>73.63</v>
       </c>
       <c r="F19" t="n">
-        <v>32.60489153862</v>
+        <v>26.67883896827698</v>
       </c>
     </row>
     <row r="20">
@@ -1298,7 +1298,7 @@
         <v>73.78</v>
       </c>
       <c r="F20" t="n">
-        <v>32.89835977554321</v>
+        <v>26.62525224685669</v>
       </c>
     </row>
     <row r="21">
@@ -1318,7 +1318,7 @@
         <v>73.2</v>
       </c>
       <c r="F21" t="n">
-        <v>33.24507308006287</v>
+        <v>26.89186120033264</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1389,7 @@
         <v>47.56</v>
       </c>
       <c r="F2" t="n">
-        <v>33.35871076583862</v>
+        <v>26.83164644241333</v>
       </c>
     </row>
     <row r="3">
@@ -1409,7 +1409,7 @@
         <v>55.53</v>
       </c>
       <c r="F3" t="n">
-        <v>32.56006693840027</v>
+        <v>26.60200762748718</v>
       </c>
     </row>
     <row r="4">
@@ -1429,7 +1429,7 @@
         <v>58.92</v>
       </c>
       <c r="F4" t="n">
-        <v>32.62535119056702</v>
+        <v>26.5997109413147</v>
       </c>
     </row>
     <row r="5">
@@ -1449,7 +1449,7 @@
         <v>62.15</v>
       </c>
       <c r="F5" t="n">
-        <v>34.16694164276123</v>
+        <v>26.62772154808044</v>
       </c>
     </row>
     <row r="6">
@@ -1469,7 +1469,7 @@
         <v>64.51000000000001</v>
       </c>
       <c r="F6" t="n">
-        <v>32.59046983718872</v>
+        <v>26.75187754631042</v>
       </c>
     </row>
     <row r="7">
@@ -1489,7 +1489,7 @@
         <v>65.45</v>
       </c>
       <c r="F7" t="n">
-        <v>33.06958818435669</v>
+        <v>26.6960756778717</v>
       </c>
     </row>
     <row r="8">
@@ -1509,7 +1509,7 @@
         <v>67.18000000000001</v>
       </c>
       <c r="F8" t="n">
-        <v>32.50585079193115</v>
+        <v>26.58644080162048</v>
       </c>
     </row>
     <row r="9">
@@ -1529,7 +1529,7 @@
         <v>68.5</v>
       </c>
       <c r="F9" t="n">
-        <v>33.11872529983521</v>
+        <v>26.51874613761902</v>
       </c>
     </row>
     <row r="10">
@@ -1549,7 +1549,7 @@
         <v>68.73</v>
       </c>
       <c r="F10" t="n">
-        <v>32.63175201416016</v>
+        <v>26.54516506195068</v>
       </c>
     </row>
     <row r="11">
@@ -1569,7 +1569,7 @@
         <v>70.36</v>
       </c>
       <c r="F11" t="n">
-        <v>32.36810898780823</v>
+        <v>26.81162762641907</v>
       </c>
     </row>
     <row r="12">
@@ -1589,7 +1589,7 @@
         <v>70.44</v>
       </c>
       <c r="F12" t="n">
-        <v>32.36715388298035</v>
+        <v>26.67332696914673</v>
       </c>
     </row>
     <row r="13">
@@ -1609,7 +1609,7 @@
         <v>71.09</v>
       </c>
       <c r="F13" t="n">
-        <v>32.13305282592773</v>
+        <v>26.55418825149536</v>
       </c>
     </row>
     <row r="14">
@@ -1629,7 +1629,7 @@
         <v>71.91</v>
       </c>
       <c r="F14" t="n">
-        <v>32.28047847747803</v>
+        <v>26.56037092208862</v>
       </c>
     </row>
     <row r="15">
@@ -1649,7 +1649,7 @@
         <v>71.89</v>
       </c>
       <c r="F15" t="n">
-        <v>32.34851241111755</v>
+        <v>26.50875878334045</v>
       </c>
     </row>
     <row r="16">
@@ -1669,7 +1669,7 @@
         <v>73.06</v>
       </c>
       <c r="F16" t="n">
-        <v>32.22534203529358</v>
+        <v>26.41753149032593</v>
       </c>
     </row>
     <row r="17">
@@ -1689,7 +1689,7 @@
         <v>73.52</v>
       </c>
       <c r="F17" t="n">
-        <v>32.04878711700439</v>
+        <v>26.82300734519958</v>
       </c>
     </row>
     <row r="18">
@@ -1709,7 +1709,7 @@
         <v>74.25</v>
       </c>
       <c r="F18" t="n">
-        <v>32.12067079544067</v>
+        <v>26.60252118110657</v>
       </c>
     </row>
     <row r="19">
@@ -1729,7 +1729,7 @@
         <v>74.48999999999999</v>
       </c>
       <c r="F19" t="n">
-        <v>32.30143094062805</v>
+        <v>26.63367104530334</v>
       </c>
     </row>
     <row r="20">
@@ -1749,7 +1749,7 @@
         <v>74.06</v>
       </c>
       <c r="F20" t="n">
-        <v>32.09705209732056</v>
+        <v>26.65050005912781</v>
       </c>
     </row>
     <row r="21">
@@ -1769,7 +1769,7 @@
         <v>73.38</v>
       </c>
       <c r="F21" t="n">
-        <v>32.59001851081848</v>
+        <v>26.902508020401</v>
       </c>
     </row>
   </sheetData>
@@ -1840,7 +1840,7 @@
         <v>48.16</v>
       </c>
       <c r="F2" t="n">
-        <v>32.30961608886719</v>
+        <v>26.88038873672485</v>
       </c>
     </row>
     <row r="3">
@@ -1860,7 +1860,7 @@
         <v>54.03</v>
       </c>
       <c r="F3" t="n">
-        <v>32.42212200164795</v>
+        <v>26.60947751998901</v>
       </c>
     </row>
     <row r="4">
@@ -1880,7 +1880,7 @@
         <v>57.94</v>
       </c>
       <c r="F4" t="n">
-        <v>32.27682995796204</v>
+        <v>26.7687623500824</v>
       </c>
     </row>
     <row r="5">
@@ -1900,7 +1900,7 @@
         <v>60.32</v>
       </c>
       <c r="F5" t="n">
-        <v>32.00633978843689</v>
+        <v>26.69063496589661</v>
       </c>
     </row>
     <row r="6">
@@ -1920,7 +1920,7 @@
         <v>63.59</v>
       </c>
       <c r="F6" t="n">
-        <v>32.04639220237732</v>
+        <v>26.67008781433105</v>
       </c>
     </row>
     <row r="7">
@@ -1940,7 +1940,7 @@
         <v>66.28</v>
       </c>
       <c r="F7" t="n">
-        <v>32.09815812110901</v>
+        <v>26.40389919281006</v>
       </c>
     </row>
     <row r="8">
@@ -1960,7 +1960,7 @@
         <v>67.09999999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>32.15049624443054</v>
+        <v>26.52817678451538</v>
       </c>
     </row>
     <row r="9">
@@ -1980,7 +1980,7 @@
         <v>66.40000000000001</v>
       </c>
       <c r="F9" t="n">
-        <v>32.16439056396484</v>
+        <v>26.5012469291687</v>
       </c>
     </row>
     <row r="10">
@@ -2000,7 +2000,7 @@
         <v>67.55</v>
       </c>
       <c r="F10" t="n">
-        <v>32.42030811309814</v>
+        <v>26.53488731384277</v>
       </c>
     </row>
     <row r="11">
@@ -2020,7 +2020,7 @@
         <v>67.27</v>
       </c>
       <c r="F11" t="n">
-        <v>32.24553561210632</v>
+        <v>26.84052920341492</v>
       </c>
     </row>
     <row r="12">
@@ -2040,7 +2040,7 @@
         <v>70.09</v>
       </c>
       <c r="F12" t="n">
-        <v>31.99336957931519</v>
+        <v>26.64801478385925</v>
       </c>
     </row>
     <row r="13">
@@ -2060,7 +2060,7 @@
         <v>70.7</v>
       </c>
       <c r="F13" t="n">
-        <v>32.11574578285217</v>
+        <v>26.70173811912537</v>
       </c>
     </row>
     <row r="14">
@@ -2080,7 +2080,7 @@
         <v>70.72</v>
       </c>
       <c r="F14" t="n">
-        <v>32.21752262115479</v>
+        <v>26.55263805389404</v>
       </c>
     </row>
     <row r="15">
@@ -2100,7 +2100,7 @@
         <v>71.56</v>
       </c>
       <c r="F15" t="n">
-        <v>32.10472226142883</v>
+        <v>26.56175518035889</v>
       </c>
     </row>
     <row r="16">
@@ -2120,7 +2120,7 @@
         <v>71.56</v>
       </c>
       <c r="F16" t="n">
-        <v>31.95874547958374</v>
+        <v>26.61720991134644</v>
       </c>
     </row>
     <row r="17">
@@ -2140,7 +2140,7 @@
         <v>72.67</v>
       </c>
       <c r="F17" t="n">
-        <v>32.46766710281372</v>
+        <v>26.48142051696777</v>
       </c>
     </row>
     <row r="18">
@@ -2160,7 +2160,7 @@
         <v>72.59999999999999</v>
       </c>
       <c r="F18" t="n">
-        <v>32.07568073272705</v>
+        <v>26.49393177032471</v>
       </c>
     </row>
     <row r="19">
@@ -2180,7 +2180,7 @@
         <v>71.75</v>
       </c>
       <c r="F19" t="n">
-        <v>32.30819511413574</v>
+        <v>26.48260402679444</v>
       </c>
     </row>
     <row r="20">
@@ -2200,7 +2200,7 @@
         <v>73.14</v>
       </c>
       <c r="F20" t="n">
-        <v>31.9996612071991</v>
+        <v>26.63510775566101</v>
       </c>
     </row>
     <row r="21">
@@ -2220,7 +2220,7 @@
         <v>73.77</v>
       </c>
       <c r="F21" t="n">
-        <v>32.22734045982361</v>
+        <v>26.8668487071991</v>
       </c>
     </row>
   </sheetData>
@@ -2291,7 +2291,7 @@
         <v>47.42</v>
       </c>
       <c r="F2" t="n">
-        <v>32.0508668422699</v>
+        <v>26.92673206329346</v>
       </c>
     </row>
     <row r="3">
@@ -2311,7 +2311,7 @@
         <v>53.81</v>
       </c>
       <c r="F3" t="n">
-        <v>32.13609457015991</v>
+        <v>26.6506085395813</v>
       </c>
     </row>
     <row r="4">
@@ -2331,7 +2331,7 @@
         <v>59.31</v>
       </c>
       <c r="F4" t="n">
-        <v>32.10563516616821</v>
+        <v>26.61904692649841</v>
       </c>
     </row>
     <row r="5">
@@ -2351,7 +2351,7 @@
         <v>61.49</v>
       </c>
       <c r="F5" t="n">
-        <v>32.39140176773071</v>
+        <v>26.65190100669861</v>
       </c>
     </row>
     <row r="6">
@@ -2371,7 +2371,7 @@
         <v>63.4</v>
       </c>
       <c r="F6" t="n">
-        <v>32.23519110679626</v>
+        <v>26.62372183799744</v>
       </c>
     </row>
     <row r="7">
@@ -2391,7 +2391,7 @@
         <v>65.86</v>
       </c>
       <c r="F7" t="n">
-        <v>32.04871320724487</v>
+        <v>26.67050194740296</v>
       </c>
     </row>
     <row r="8">
@@ -2411,7 +2411,7 @@
         <v>66.25</v>
       </c>
       <c r="F8" t="n">
-        <v>32.01001405715942</v>
+        <v>26.67687273025513</v>
       </c>
     </row>
     <row r="9">
@@ -2431,7 +2431,7 @@
         <v>66.70999999999999</v>
       </c>
       <c r="F9" t="n">
-        <v>32.06966233253479</v>
+        <v>26.6266610622406</v>
       </c>
     </row>
     <row r="10">
@@ -2451,7 +2451,7 @@
         <v>68.47</v>
       </c>
       <c r="F10" t="n">
-        <v>32.13233041763306</v>
+        <v>26.63897323608398</v>
       </c>
     </row>
     <row r="11">
@@ -2471,7 +2471,7 @@
         <v>68.72</v>
       </c>
       <c r="F11" t="n">
-        <v>31.99724221229553</v>
+        <v>26.90861678123474</v>
       </c>
     </row>
     <row r="12">
@@ -2491,7 +2491,7 @@
         <v>69.81999999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>32.1812686920166</v>
+        <v>26.5458459854126</v>
       </c>
     </row>
     <row r="13">
@@ -2511,7 +2511,7 @@
         <v>69.95</v>
       </c>
       <c r="F13" t="n">
-        <v>32.11719489097595</v>
+        <v>26.66955590248108</v>
       </c>
     </row>
     <row r="14">
@@ -2531,7 +2531,7 @@
         <v>70.94</v>
       </c>
       <c r="F14" t="n">
-        <v>31.46775364875793</v>
+        <v>26.59504294395447</v>
       </c>
     </row>
     <row r="15">
@@ -2551,7 +2551,7 @@
         <v>71.38</v>
       </c>
       <c r="F15" t="n">
-        <v>30.74691224098206</v>
+        <v>26.71591520309448</v>
       </c>
     </row>
     <row r="16">
@@ -2571,7 +2571,7 @@
         <v>71.76000000000001</v>
       </c>
       <c r="F16" t="n">
-        <v>31.03618264198303</v>
+        <v>26.56165313720703</v>
       </c>
     </row>
     <row r="17">
@@ -2591,7 +2591,7 @@
         <v>70.95</v>
       </c>
       <c r="F17" t="n">
-        <v>30.93668508529663</v>
+        <v>26.67468285560608</v>
       </c>
     </row>
     <row r="18">
@@ -2611,7 +2611,7 @@
         <v>72.15000000000001</v>
       </c>
       <c r="F18" t="n">
-        <v>31.16248941421509</v>
+        <v>26.70881152153015</v>
       </c>
     </row>
     <row r="19">
@@ -2631,7 +2631,7 @@
         <v>72.86</v>
       </c>
       <c r="F19" t="n">
-        <v>31.06265044212341</v>
+        <v>26.64816379547119</v>
       </c>
     </row>
     <row r="20">
@@ -2651,7 +2651,7 @@
         <v>73.45</v>
       </c>
       <c r="F20" t="n">
-        <v>31.18937849998474</v>
+        <v>26.64202523231506</v>
       </c>
     </row>
     <row r="21">
@@ -2671,7 +2671,7 @@
         <v>73.41</v>
       </c>
       <c r="F21" t="n">
-        <v>31.30718874931335</v>
+        <v>26.78550815582276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>